<commit_message>
Heavily revised 35Ca->35K EC decay set
</commit_message>
<xml_diff>
--- a/35K EC, 36Ca ECP.xlsx
+++ b/35K EC, 36Ca ECP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77CA6CD-BD27-4837-B3E0-155004A61CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1E9D4E-CEC8-4BC1-B552-45A28D75C0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10476" yWindow="312" windowWidth="11436" windowHeight="12000" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
   </bookViews>
   <sheets>
     <sheet name="36 ECP" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="117">
   <si>
     <t>Ip</t>
   </si>
@@ -284,9 +284,6 @@
     <t>1993AU07</t>
   </si>
   <si>
-    <t>Used</t>
-  </si>
-  <si>
     <t>Min</t>
   </si>
   <si>
@@ -359,7 +356,37 @@
     <t>35K</t>
   </si>
   <si>
-    <t>6983(22)</t>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>Used in 2025</t>
+  </si>
+  <si>
+    <t>5.4(9)</t>
+  </si>
+  <si>
+    <t>1.0(4)</t>
+  </si>
+  <si>
+    <t>2.0(7)</t>
+  </si>
+  <si>
+    <t>IAS</t>
+  </si>
+  <si>
+    <t>1985Ay01</t>
+  </si>
+  <si>
+    <t>2p₁</t>
+  </si>
+  <si>
+    <t>6783(22)</t>
   </si>
 </sst>
 </file>
@@ -370,7 +397,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +524,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0066"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -519,7 +566,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -632,6 +679,18 @@
     <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,6 +700,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0066"/>
       <color rgb="FFA50021"/>
       <color rgb="FF9933FF"/>
       <color rgb="FF660033"/>
@@ -650,7 +710,6 @@
       <color rgb="FF993300"/>
       <color rgb="FFD9F1FF"/>
       <color rgb="FFFFD9B3"/>
-      <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2495,7 +2554,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I2" s="20">
         <v>7527</v>
@@ -2921,10 +2980,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0A5003-67F5-4A2F-AC32-71311414C574}">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37:O37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="11.4" x14ac:dyDescent="0.3"/>
@@ -2934,8 +2993,8 @@
     <col min="3" max="3" width="7.21875" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="3.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="5" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.21875" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.109375" style="16" bestFit="1" customWidth="1"/>
@@ -2948,7 +3007,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="12" x14ac:dyDescent="0.3">
       <c r="D1" s="16" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>70</v>
@@ -3018,7 +3077,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>27</v>
@@ -3054,7 +3113,7 @@
         <v>78</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3099,7 +3158,7 @@
         <v>5.1712875121068231</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3147,7 +3206,7 @@
         <v>13.39169034297816</v>
       </c>
       <c r="O7" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3195,7 +3254,7 @@
         <v>25.740150802235007</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3243,7 +3302,7 @@
         <v>37.062196391796363</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3291,7 +3350,7 @@
         <v>73.089945535677515</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3324,7 +3383,7 @@
         <v>49.411764705882355</v>
       </c>
       <c r="I11" s="19">
-        <f>$F11+$F$1</f>
+        <f t="shared" ref="I11:I17" si="6">$F11+$F$1</f>
         <v>4788.0117647058823</v>
       </c>
       <c r="J11" s="19"/>
@@ -3339,7 +3398,7 @@
         <v>49.414294403031612</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3372,7 +3431,7 @@
         <v>39.117647058823529</v>
       </c>
       <c r="I12" s="19">
-        <f>$F12+$F$1</f>
+        <f t="shared" si="6"/>
         <v>4977.4235294117643</v>
       </c>
       <c r="J12" s="19"/>
@@ -3387,7 +3446,7 @@
         <v>39.120842417037558</v>
       </c>
       <c r="O12" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3420,7 +3479,7 @@
         <v>73.088235294117652</v>
       </c>
       <c r="I13" s="19">
-        <f>$F13+$F$1</f>
+        <f t="shared" si="6"/>
         <v>5249.1882352941184</v>
       </c>
       <c r="J13" s="19"/>
@@ -3435,7 +3494,7 @@
         <v>73.089945535677515</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3468,7 +3527,7 @@
         <v>49.411764705882355</v>
       </c>
       <c r="I14" s="19">
-        <f>$F14+$F$1</f>
+        <f t="shared" si="6"/>
         <v>5533.3058823529418</v>
       </c>
       <c r="J14" s="19"/>
@@ -3483,7 +3542,7 @@
         <v>49.414294403031612</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3516,7 +3575,7 @@
         <v>49.411764705882355</v>
       </c>
       <c r="I15" s="19">
-        <f>$F15+$F$1</f>
+        <f t="shared" si="6"/>
         <v>5710.3647058823526</v>
       </c>
       <c r="J15" s="19"/>
@@ -3531,7 +3590,7 @@
         <v>49.414294403031612</v>
       </c>
       <c r="O15" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
@@ -3564,7 +3623,7 @@
         <v>38.088235294117645</v>
       </c>
       <c r="I16" s="19">
-        <f>$F16+$F$1</f>
+        <f t="shared" si="6"/>
         <v>5864.7764705882364</v>
       </c>
       <c r="J16" s="19"/>
@@ -3579,10 +3638,10 @@
         <v>38.09151700602208</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>15</v>
       </c>
@@ -3627,15 +3686,15 @@
         <v>61.766729658721317</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>61</v>
@@ -3644,12 +3703,12 @@
         <v>37</v>
       </c>
       <c r="E18" s="16" t="str">
-        <f t="shared" ref="E18" si="6">LEFT(B18,4)</f>
-        <v>6983</v>
+        <f t="shared" ref="E18" si="7">LEFT(B18,4)</f>
+        <v>6783</v>
       </c>
       <c r="F18" s="16">
         <f>E18/34*35</f>
-        <v>7188.3823529411766</v>
+        <v>6982.5</v>
       </c>
       <c r="G18" s="16" t="str">
         <f t="shared" si="5"/>
@@ -3660,23 +3719,26 @@
         <v>22.647058823529413</v>
       </c>
       <c r="I18" s="19"/>
-      <c r="J18" s="16">
-        <f>$E18+$F$1+J$5</f>
-        <v>9157.7000000000007</v>
-      </c>
-      <c r="M18" s="34">
+      <c r="J18" s="19">
+        <f>$F18+$F$1+J$5</f>
+        <v>9157.2000000000007</v>
+      </c>
+      <c r="M18" s="38">
         <f>MAX(I18:L18)</f>
-        <v>9157.7000000000007</v>
-      </c>
-      <c r="N18" s="34">
+        <v>9157.2000000000007</v>
+      </c>
+      <c r="N18" s="38">
         <f t="shared" si="4"/>
         <v>22.652577631616261</v>
       </c>
-      <c r="O18" s="35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="O18" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="P18" s="39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>19</v>
       </c>
@@ -3706,22 +3768,25 @@
         <v>91.617647058823536</v>
       </c>
       <c r="I19" s="19">
-        <f>$E19/34*35+$F$1</f>
+        <f>$F19+$F$1</f>
         <v>9144.4823529411769</v>
       </c>
-      <c r="M19" s="34">
+      <c r="M19" s="38">
         <f t="shared" si="3"/>
         <v>9144.4823529411769</v>
       </c>
-      <c r="N19" s="34">
+      <c r="N19" s="38">
         <f t="shared" si="4"/>
         <v>91.61901141463575</v>
       </c>
-      <c r="O19" s="35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O19" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="P19" s="39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="H20" s="19"/>
@@ -3729,7 +3794,7 @@
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
     </row>
-    <row r="21" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>4</v>
       </c>
@@ -3756,18 +3821,18 @@
         <f>$F21+$F$1+J$5</f>
         <v>5208.376470588235</v>
       </c>
-      <c r="M21" s="24">
-        <f t="shared" si="3"/>
+      <c r="P21" s="24">
+        <f>MAX(I21:L21)</f>
         <v>5208.376470588235</v>
       </c>
-      <c r="N21" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="O21" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="Q21" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="R21" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <v>16</v>
       </c>
@@ -3794,18 +3859,18 @@
         <v>6242.5705882352941</v>
       </c>
       <c r="J22" s="19"/>
-      <c r="M22" s="21">
-        <f t="shared" si="3"/>
+      <c r="P22" s="21">
+        <f>MAX(I22:L22)</f>
         <v>6242.5705882352941</v>
       </c>
-      <c r="N22" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="O22" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="Q22" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="R22" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>18</v>
       </c>
@@ -3832,18 +3897,18 @@
         <v>7424.3352941176481</v>
       </c>
       <c r="J23" s="19"/>
-      <c r="M23" s="28">
-        <f t="shared" si="3"/>
+      <c r="P23" s="28">
+        <f>MAX(I23:L23)</f>
         <v>7424.3352941176481</v>
       </c>
-      <c r="N23" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="O23" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="Q23" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="R23" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>4</v>
       </c>
@@ -3868,19 +3933,19 @@
         <f>$F24+$F$1+J$5</f>
         <v>5777.6411764705881</v>
       </c>
-      <c r="M24" s="24">
-        <f t="shared" si="3"/>
+      <c r="S24" s="24">
+        <f>MAX(I24:L24)</f>
         <v>5777.6411764705881</v>
       </c>
-      <c r="N24" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="O24" s="16" t="str">
-        <f>O21</f>
+      <c r="T24" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="U24" s="16" t="str">
+        <f>R21</f>
         <v>L8</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <v>16</v>
       </c>
@@ -3894,30 +3959,30 @@
         <v>32</v>
       </c>
       <c r="E25" s="19" t="str">
-        <f t="shared" ref="E25:E26" si="7">RIGHT(B25,4)</f>
+        <f t="shared" ref="E25" si="8">RIGHT(B25,4)</f>
         <v>6649</v>
       </c>
       <c r="F25" s="16">
-        <f t="shared" ref="F25:F26" si="8">E25/34*35</f>
+        <f t="shared" ref="F25:F26" si="9">E25/34*35</f>
         <v>6844.5588235294117</v>
       </c>
       <c r="I25" s="19">
         <f>$F25+$F$1</f>
         <v>6928.1588235294121</v>
       </c>
-      <c r="M25" s="21">
-        <f t="shared" si="3"/>
+      <c r="S25" s="21">
+        <f>MAX(I25:L25)</f>
         <v>6928.1588235294121</v>
       </c>
-      <c r="N25" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="O25" s="16" t="str">
-        <f t="shared" ref="O25:O26" si="9">O22</f>
+      <c r="T25" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="U25" s="16" t="str">
+        <f>R22</f>
         <v>L16</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>18</v>
       </c>
@@ -3935,26 +4000,26 @@
         <v>7887</v>
       </c>
       <c r="F26" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8118.9705882352937</v>
       </c>
       <c r="I26" s="19">
         <f>$F26+$F$1</f>
         <v>8202.5705882352941</v>
       </c>
-      <c r="M26" s="28">
-        <f t="shared" si="3"/>
+      <c r="S26" s="28">
+        <f>MAX(I26:L26)</f>
         <v>8202.5705882352941</v>
       </c>
-      <c r="N26" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="O26" s="16" t="str">
-        <f t="shared" si="9"/>
+      <c r="T26" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="U26" s="16" t="str">
+        <f>R23</f>
         <v>L17</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A27" s="16">
         <v>4</v>
       </c>
@@ -3981,19 +4046,19 @@
         <f>$F27+$F$1+J$5</f>
         <v>5493.0088235294115</v>
       </c>
-      <c r="M27" s="24">
+      <c r="M27" s="37">
         <f>MAX(I27:L27)</f>
         <v>5493.0088235294115</v>
       </c>
-      <c r="N27" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="O27" s="16" t="str">
-        <f>O21</f>
+      <c r="N27" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="O27" s="36" t="str">
+        <f>R21</f>
         <v>L8</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>16</v>
       </c>
@@ -4020,19 +4085,19 @@
         <v>6585.3647058823526</v>
       </c>
       <c r="J28" s="19"/>
-      <c r="M28" s="21">
+      <c r="M28" s="40">
         <f>MAX(I28:L28)</f>
         <v>6585.3647058823526</v>
       </c>
-      <c r="N28" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="O28" s="16" t="str">
-        <f t="shared" ref="O28:O29" si="10">O22</f>
+      <c r="N28" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="O28" s="36" t="str">
+        <f>R22</f>
         <v>L16</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A29" s="16">
         <v>18</v>
       </c>
@@ -4059,19 +4124,24 @@
         <v>7813.4529411764706</v>
       </c>
       <c r="J29" s="19"/>
-      <c r="M29" s="28">
+      <c r="M29" s="41">
         <f>MAX(I29:L29)</f>
         <v>7813.4529411764706</v>
       </c>
-      <c r="N29" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="O29" s="16" t="str">
-        <f t="shared" si="10"/>
+      <c r="N29" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="O29" s="36" t="str">
+        <f>R23</f>
         <v>L17</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="12" x14ac:dyDescent="0.3">
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+    </row>
+    <row r="31" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
         <v>2</v>
       </c>
@@ -4092,34 +4162,61 @@
         <f>E31/34*35</f>
         <v>1965.1470588235295</v>
       </c>
-      <c r="G31" s="19"/>
+      <c r="G31" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>106</v>
+      </c>
       <c r="I31" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J31" s="19">
         <f>$F31+$F$1+J$5</f>
         <v>4139.8470588235296</v>
       </c>
       <c r="K31" s="19">
-        <f>$F31+$F$1+K$5</f>
+        <f t="shared" ref="J31:L33" si="10">$F31+$F$1+K$5</f>
         <v>5336.447058823529</v>
       </c>
       <c r="L31" s="19">
-        <f>$F31+$F$1+L$5</f>
+        <f t="shared" si="10"/>
         <v>5921.7470588235301</v>
       </c>
-      <c r="M31" s="24">
+      <c r="M31" s="37">
+        <f>J33</f>
+        <v>4519.7</v>
+      </c>
+      <c r="N31" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="O31" s="36" t="str">
+        <f>R31</f>
+        <v>L4</v>
+      </c>
+      <c r="P31" s="24">
         <f>J31</f>
         <v>4139.8470588235296</v>
       </c>
-      <c r="N31" s="23" t="s">
+      <c r="Q31" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="R31" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="S31" s="24">
+        <f>J32</f>
+        <v>4899.552941176471</v>
+      </c>
+      <c r="T31" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="O31" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="U31" s="16" t="str">
+        <f>R31</f>
+        <v>L4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>2</v>
       </c>
@@ -4140,33 +4237,61 @@
         <f>E32/34*35</f>
         <v>2724.8529411764707</v>
       </c>
+      <c r="G32" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>107</v>
+      </c>
       <c r="I32" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J32" s="19">
+        <f t="shared" si="10"/>
+        <v>4899.552941176471</v>
+      </c>
+      <c r="K32" s="19">
+        <f t="shared" si="10"/>
+        <v>6096.1529411764704</v>
+      </c>
+      <c r="L32" s="19">
+        <f t="shared" si="10"/>
+        <v>6681.4529411764706</v>
+      </c>
+      <c r="M32" s="40">
+        <f>K33</f>
+        <v>5716.2999999999993</v>
+      </c>
+      <c r="N32" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="J32" s="19">
-        <f>$F32+$F$1+J$5</f>
-        <v>4899.552941176471</v>
-      </c>
-      <c r="K32" s="19">
-        <f>$F32+$F$1+K$5</f>
-        <v>6096.1529411764704</v>
-      </c>
-      <c r="L32" s="19">
-        <f>$F32+$F$1+L$5</f>
-        <v>6681.4529411764706</v>
-      </c>
-      <c r="M32" s="21">
+      <c r="O32" s="36" t="str">
+        <f>R32</f>
+        <v>L11</v>
+      </c>
+      <c r="P32" s="21">
         <f>K31</f>
         <v>5336.447058823529</v>
       </c>
-      <c r="N32" s="20" t="s">
+      <c r="Q32" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="R32" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="S32" s="21">
+        <f>K32</f>
+        <v>6096.1529411764704</v>
+      </c>
+      <c r="T32" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="O32" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="U32" s="16" t="str">
+        <f>R32</f>
+        <v>L11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>2</v>
       </c>
@@ -4187,197 +4312,188 @@
         <f>E33/34*35</f>
         <v>2345</v>
       </c>
+      <c r="G33" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>108</v>
+      </c>
       <c r="I33" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J33" s="19">
-        <f>$F33+$F$1+J$5</f>
+        <f t="shared" si="10"/>
         <v>4519.7</v>
       </c>
       <c r="K33" s="19">
-        <f>$F33+$F$1+K$5</f>
+        <f t="shared" si="10"/>
         <v>5716.2999999999993</v>
       </c>
       <c r="L33" s="19">
-        <f>$F33+$F$1+L$5</f>
+        <f t="shared" si="10"/>
         <v>6301.6</v>
       </c>
-      <c r="M33" s="28">
+      <c r="M33" s="41">
+        <f>L33</f>
+        <v>6301.6</v>
+      </c>
+      <c r="N33" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="O33" s="36" t="str">
+        <f>R33</f>
+        <v>L14</v>
+      </c>
+      <c r="P33" s="28">
         <f>L31</f>
         <v>5921.7470588235301</v>
       </c>
-      <c r="N33" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="O33" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M34" s="24">
-        <f>J32</f>
-        <v>4899.552941176471</v>
-      </c>
-      <c r="N34" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="O34" s="16" t="str">
-        <f>O31</f>
-        <v>L4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M35" s="21">
-        <f>K32</f>
-        <v>6096.1529411764704</v>
-      </c>
-      <c r="N35" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="O35" s="16" t="str">
-        <f t="shared" ref="O35:O36" si="11">O32</f>
-        <v>L11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M36" s="28">
+      <c r="Q33" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="R33" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="S33" s="28">
         <f>L32</f>
         <v>6681.4529411764706</v>
       </c>
-      <c r="N36" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="O36" s="16" t="str">
-        <f t="shared" si="11"/>
+      <c r="T33" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="U33" s="16" t="str">
+        <f>R33</f>
         <v>L14</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="12" x14ac:dyDescent="0.3">
-      <c r="M37" s="37">
-        <f>J33</f>
-        <v>4519.7</v>
-      </c>
-      <c r="N37" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="O37" s="36" t="str">
-        <f>O31</f>
-        <v>L4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M38" s="21">
-        <f>K33</f>
-        <v>5716.2999999999993</v>
-      </c>
-      <c r="N38" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="O38" s="16" t="str">
-        <f t="shared" ref="O38:O39" si="12">O32</f>
-        <v>L11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M39" s="28">
-        <f>L33</f>
-        <v>6301.6</v>
-      </c>
-      <c r="N39" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="O39" s="16" t="str">
-        <f t="shared" si="12"/>
-        <v>L14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="12" x14ac:dyDescent="0.3">
-      <c r="D40" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E40" s="16" t="s">
+    <row r="36" spans="1:21" ht="12" x14ac:dyDescent="0.3">
+      <c r="D36" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="36">
-        <f>F41</f>
+      <c r="F36" s="36">
+        <f>F37</f>
         <v>4747.5</v>
       </c>
-      <c r="G40" s="36">
-        <f>G41</f>
+      <c r="G36" s="36">
+        <f>G37</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="D41" s="32" t="s">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D37" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="32" t="s">
+      <c r="E37" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="32">
+      <c r="F37" s="32">
         <v>4747.5</v>
       </c>
-      <c r="G41" s="32">
+      <c r="G37" s="32">
         <v>0.6</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="D42" s="32" t="s">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D38" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="32" t="s">
+      <c r="E38" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F42" s="32">
+      <c r="F38" s="32">
         <v>4742</v>
       </c>
-      <c r="G42" s="32">
+      <c r="G38" s="32">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="16">
+    <row r="39" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
         <v>8</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B39" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C39" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D39" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="16" t="str">
-        <f>LEFT(B43,4)</f>
+      <c r="E39" s="16" t="str">
+        <f>LEFT(B39,4)</f>
         <v>4305</v>
       </c>
-      <c r="F43" s="16">
-        <f>E43/34*35</f>
+      <c r="F39" s="16">
+        <f>E39/34*35</f>
         <v>4431.6176470588234</v>
       </c>
-      <c r="G43" s="16" t="str">
-        <f>MID(B43,6,2)</f>
+      <c r="G39" s="16" t="str">
+        <f>MID(B39,6,2)</f>
         <v>26</v>
       </c>
-      <c r="H43" s="19">
-        <f>G43/34*35</f>
+      <c r="H39" s="19">
+        <f>G39/34*35</f>
         <v>26.764705882352938</v>
       </c>
-      <c r="I43" s="19">
-        <f>$F43+$F$40+7</f>
+      <c r="I39" s="19">
+        <f>$F39+$F$36+7</f>
         <v>9186.1176470588234</v>
       </c>
-      <c r="M43" s="34">
-        <f>MAX(I43:L43)</f>
+      <c r="M39" s="38">
+        <f>MAX(I39:L39)</f>
         <v>9186.1176470588234</v>
       </c>
-      <c r="N43" s="34">
-        <f>SQRT($H43^2+G$40^2)</f>
+      <c r="N39" s="38">
+        <f>SQRT($H39^2+G$36^2)</f>
         <v>26.771430312347114</v>
       </c>
-      <c r="O43" s="35" t="s">
-        <v>104</v>
+      <c r="O39" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="P39" s="39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B40" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="16">
+        <v>4089</v>
+      </c>
+      <c r="F40" s="16">
+        <v>4311</v>
+      </c>
+      <c r="G40" s="16">
+        <v>30</v>
+      </c>
+      <c r="H40" s="19">
+        <v>40</v>
+      </c>
+      <c r="I40" s="19">
+        <f>$F40+$F$36</f>
+        <v>9058.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="B41" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="16">
+        <v>3287</v>
+      </c>
+      <c r="G41" s="16">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add consistency check outputs for 35K dataset
- Generated multiple output files for consistency checks including:
  - `35.fed`: Feeding gammas of levels
  - `35.fmt`: ENSDF check for format errors and warnings
  - `35.gam`: Gammas ordered by gamma energies
  - `35.gle`: Gammas ordered by level energies
  - `35.lev`: Levels data with detailed statistics
  - `35.mrg`: Original lines grouped by level and gamma energies
  - `35.wrn`: XREF warnings
  - `35.xrf`: Tentative adopted levels with new XREF flags
  - `35_keynumber.rpt`: Keynumbers check report with no errors found

- All files generated on Mon 05/05/2025 at 07:26:09 PM EDT with respective versions.
</commit_message>
<xml_diff>
--- a/35K EC, 36Ca ECP.xlsx
+++ b/35K EC, 36Ca ECP.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1E9D4E-CEC8-4BC1-B552-45A28D75C0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DE6AC4-BF12-44CD-A8B0-98F8F11A7B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
+    <workbookView xWindow="10272" yWindow="-96" windowWidth="11436" windowHeight="12000" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
   </bookViews>
   <sheets>
-    <sheet name="36 ECP" sheetId="1" r:id="rId1"/>
-    <sheet name="35K EC" sheetId="2" r:id="rId2"/>
-    <sheet name="35Ca EC" sheetId="3" r:id="rId3"/>
+    <sheet name="36Ca" sheetId="1" r:id="rId1"/>
+    <sheet name="35K" sheetId="2" r:id="rId2"/>
+    <sheet name="35Ca" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="118">
   <si>
     <t>Ip</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>6783(22)</t>
+  </si>
+  <si>
+    <t>first p</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -689,6 +692,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1022,7 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FCEC0C-CCF2-405C-89E2-FB3C4ADFF355}">
   <dimension ref="A1:AG47"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -2980,10 +2986,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0A5003-67F5-4A2F-AC32-71311414C574}">
-  <dimension ref="A1:U41"/>
+  <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="11.4" x14ac:dyDescent="0.3"/>
@@ -3198,7 +3204,7 @@
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
       <c r="M7" s="30">
-        <f t="shared" ref="M7:M26" si="3">MAX(I7:L7)</f>
+        <f t="shared" ref="M7:M19" si="3">MAX(I7:L7)</f>
         <v>4981.9058823529413</v>
       </c>
       <c r="N7" s="30">
@@ -3383,7 +3389,7 @@
         <v>49.411764705882355</v>
       </c>
       <c r="I11" s="19">
-        <f t="shared" ref="I11:I17" si="6">$F11+$F$1</f>
+        <f t="shared" ref="I11:I16" si="6">$F11+$F$1</f>
         <v>4788.0117647058823</v>
       </c>
       <c r="J11" s="19"/>
@@ -3419,7 +3425,7 @@
         <v>4754</v>
       </c>
       <c r="F12" s="16">
-        <f t="shared" si="1"/>
+        <f>E12/34*35</f>
         <v>4893.823529411764</v>
       </c>
       <c r="G12" s="16" t="str">
@@ -3431,7 +3437,7 @@
         <v>39.117647058823529</v>
       </c>
       <c r="I12" s="19">
-        <f t="shared" si="6"/>
+        <f>$F12+$F$1</f>
         <v>4977.4235294117643</v>
       </c>
       <c r="J12" s="19"/>
@@ -4032,7 +4038,7 @@
       <c r="D27" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="42">
         <f>(LEFT(B21,4)+RIGHT(B21,4))/2</f>
         <v>3223.5</v>
       </c>
@@ -4071,7 +4077,7 @@
       <c r="D28" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="36">
         <f>(LEFT(B22,4)+RIGHT(B22,4))/2</f>
         <v>6316</v>
       </c>
@@ -4110,7 +4116,7 @@
       <c r="D29" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="36">
         <f>(LEFT(B23,4)+RIGHT(B23,4))/2</f>
         <v>7509</v>
       </c>
@@ -4247,7 +4253,7 @@
         <v>83</v>
       </c>
       <c r="J32" s="19">
-        <f t="shared" si="10"/>
+        <f>$F32+$F$1+J$5</f>
         <v>4899.552941176471</v>
       </c>
       <c r="K32" s="19">
@@ -4304,7 +4310,7 @@
       <c r="D33" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="36">
         <f>(LEFT(B33,4)+RIGHT(B33,4))/2</f>
         <v>2278</v>
       </c>
@@ -4494,6 +4500,25 @@
       </c>
       <c r="G41" s="16">
         <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B42" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" s="16">
+        <v>2213</v>
+      </c>
+      <c r="F42" s="16">
+        <f>E42/34*35</f>
+        <v>2278.088235294118</v>
+      </c>
+      <c r="I42" s="19">
+        <f>$F42+$F$1</f>
+        <v>2361.6882352941179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update nuclear data sheets for 35K, including revisions to decay modes, cross-reference flags, and energy levels. Enhanced clarity in descriptions and corrected formatting inconsistencies. Added Java command script for batch processing of ENS files to PDF conversion.
</commit_message>
<xml_diff>
--- a/35K EC, 36Ca ECP.xlsx
+++ b/35K EC, 36Ca ECP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DE6AC4-BF12-44CD-A8B0-98F8F11A7B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ACDEE0-B2AE-4E86-9941-FCD600781E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10272" yWindow="-96" windowWidth="11436" windowHeight="12000" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
+    <workbookView xWindow="11712" yWindow="-24" windowWidth="11436" windowHeight="12000" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
   </bookViews>
   <sheets>
     <sheet name="36Ca" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -695,6 +695,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2986,10 +2989,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0A5003-67F5-4A2F-AC32-71311414C574}">
-  <dimension ref="A1:U42"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="11.4" x14ac:dyDescent="0.3"/>
@@ -3011,7 +3014,7 @@
     <col min="16" max="16384" width="5.5546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12" x14ac:dyDescent="0.3">
       <c r="D1" s="16" t="s">
         <v>109</v>
       </c>
@@ -3027,7 +3030,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D2" s="33" t="s">
         <v>22</v>
       </c>
@@ -3041,7 +3044,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D3" s="33" t="s">
         <v>81</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
         <v>77</v>
       </c>
@@ -3081,7 +3084,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>104</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>1</v>
       </c>
@@ -3166,8 +3169,18 @@
       <c r="O6" s="16" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X6" s="17">
+        <v>48.5</v>
+      </c>
+      <c r="Y6" s="16">
+        <v>1.3</v>
+      </c>
+      <c r="Z6" s="17">
+        <f>X6*100/100.6</f>
+        <v>48.210735586481114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>3</v>
       </c>
@@ -3214,8 +3227,18 @@
       <c r="O7" s="31" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X7" s="17">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="16">
+        <v>5</v>
+      </c>
+      <c r="Z7" s="17">
+        <f t="shared" ref="Z7:Z19" si="5">X7*100/100.6</f>
+        <v>5.9642147117296229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>5</v>
       </c>
@@ -3237,7 +3260,7 @@
         <v>3697.6470588235293</v>
       </c>
       <c r="G8" s="16" t="str">
-        <f t="shared" ref="G8:G18" si="5">MID(B8,6,2)</f>
+        <f t="shared" ref="G8:G18" si="6">MID(B8,6,2)</f>
         <v>25</v>
       </c>
       <c r="H8" s="19">
@@ -3262,8 +3285,18 @@
       <c r="O8" s="16" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X8" s="17">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z8" s="17">
+        <f t="shared" si="5"/>
+        <v>2.9821073558648115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>6</v>
       </c>
@@ -3285,7 +3318,7 @@
         <v>3934.411764705882</v>
       </c>
       <c r="G9" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="H9" s="19">
@@ -3310,8 +3343,18 @@
       <c r="O9" s="16" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X9" s="17">
+        <v>3.8</v>
+      </c>
+      <c r="Y9" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z9" s="17">
+        <f t="shared" si="5"/>
+        <v>3.7773359840954277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>7</v>
       </c>
@@ -3333,7 +3376,7 @@
         <v>4159.8529411764712</v>
       </c>
       <c r="G10" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>71</v>
       </c>
       <c r="H10" s="19">
@@ -3358,8 +3401,18 @@
       <c r="O10" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X10" s="17">
+        <v>2.9</v>
+      </c>
+      <c r="Y10" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="17">
+        <f t="shared" si="5"/>
+        <v>2.8827037773359843</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>9</v>
       </c>
@@ -3381,7 +3434,7 @@
         <v>4704.411764705882</v>
       </c>
       <c r="G11" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="H11" s="19">
@@ -3389,7 +3442,7 @@
         <v>49.411764705882355</v>
       </c>
       <c r="I11" s="19">
-        <f t="shared" ref="I11:I16" si="6">$F11+$F$1</f>
+        <f t="shared" ref="I11:I16" si="7">$F11+$F$1</f>
         <v>4788.0117647058823</v>
       </c>
       <c r="J11" s="19"/>
@@ -3406,8 +3459,18 @@
       <c r="O11" s="16" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X11" s="17">
+        <v>2.9</v>
+      </c>
+      <c r="Y11" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="17">
+        <f t="shared" si="5"/>
+        <v>2.8827037773359843</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>10</v>
       </c>
@@ -3429,7 +3492,7 @@
         <v>4893.823529411764</v>
       </c>
       <c r="G12" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="H12" s="19">
@@ -3454,8 +3517,18 @@
       <c r="O12" s="31" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X12" s="17">
+        <v>4.2</v>
+      </c>
+      <c r="Y12" s="16">
+        <v>4</v>
+      </c>
+      <c r="Z12" s="17">
+        <f t="shared" si="5"/>
+        <v>4.174950298210736</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>11</v>
       </c>
@@ -3477,7 +3550,7 @@
         <v>5165.588235294118</v>
       </c>
       <c r="G13" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>71</v>
       </c>
       <c r="H13" s="19">
@@ -3485,7 +3558,7 @@
         <v>73.088235294117652</v>
       </c>
       <c r="I13" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5249.1882352941184</v>
       </c>
       <c r="J13" s="19"/>
@@ -3502,8 +3575,18 @@
       <c r="O13" s="16" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X13" s="17">
+        <v>3.9</v>
+      </c>
+      <c r="Y13" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="17">
+        <f t="shared" si="5"/>
+        <v>3.8767395626242549</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -3525,7 +3608,7 @@
         <v>5449.7058823529414</v>
       </c>
       <c r="G14" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="H14" s="19">
@@ -3533,7 +3616,7 @@
         <v>49.411764705882355</v>
       </c>
       <c r="I14" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5533.3058823529418</v>
       </c>
       <c r="J14" s="19"/>
@@ -3550,8 +3633,18 @@
       <c r="O14" s="16" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X14" s="43">
+        <v>0.72</v>
+      </c>
+      <c r="Y14" s="16">
+        <v>18</v>
+      </c>
+      <c r="Z14" s="43">
+        <f t="shared" si="5"/>
+        <v>0.71570576540755471</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>13</v>
       </c>
@@ -3573,7 +3666,7 @@
         <v>5626.7647058823522</v>
       </c>
       <c r="G15" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="H15" s="19">
@@ -3581,7 +3674,7 @@
         <v>49.411764705882355</v>
       </c>
       <c r="I15" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5710.3647058823526</v>
       </c>
       <c r="J15" s="19"/>
@@ -3598,8 +3691,18 @@
       <c r="O15" s="16" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X15" s="43">
+        <v>0.61</v>
+      </c>
+      <c r="Y15" s="16">
+        <v>15</v>
+      </c>
+      <c r="Z15" s="43">
+        <f t="shared" si="5"/>
+        <v>0.60636182902584501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <v>14</v>
       </c>
@@ -3621,7 +3724,7 @@
         <v>5781.176470588236</v>
       </c>
       <c r="G16" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="H16" s="19">
@@ -3629,7 +3732,7 @@
         <v>38.088235294117645</v>
       </c>
       <c r="I16" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5864.7764705882364</v>
       </c>
       <c r="J16" s="19"/>
@@ -3646,8 +3749,18 @@
       <c r="O16" s="16" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X16" s="43">
+        <v>1.43</v>
+      </c>
+      <c r="Y16" s="16">
+        <v>17</v>
+      </c>
+      <c r="Z16" s="43">
+        <f t="shared" si="5"/>
+        <v>1.4214711729622267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>15</v>
       </c>
@@ -3694,8 +3807,18 @@
       <c r="O17" s="16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X17" s="43">
+        <v>1.4</v>
+      </c>
+      <c r="Y17" s="16">
+        <v>19</v>
+      </c>
+      <c r="Z17" s="43">
+        <f t="shared" si="5"/>
+        <v>1.3916500994035785</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
         <v>17</v>
       </c>
@@ -3709,7 +3832,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="16" t="str">
-        <f t="shared" ref="E18" si="7">LEFT(B18,4)</f>
+        <f t="shared" ref="E18" si="8">LEFT(B18,4)</f>
         <v>6783</v>
       </c>
       <c r="F18" s="16">
@@ -3717,7 +3840,7 @@
         <v>6982.5</v>
       </c>
       <c r="G18" s="16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="H18" s="19">
@@ -3743,8 +3866,18 @@
       <c r="P18" s="39" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X18" s="17">
+        <v>3.8</v>
+      </c>
+      <c r="Y18" s="16">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="17">
+        <f t="shared" si="5"/>
+        <v>3.7773359840954277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>19</v>
       </c>
@@ -3791,16 +3924,28 @@
       <c r="P19" s="39" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="X19" s="43">
+        <v>0.41</v>
+      </c>
+      <c r="Y19" s="16">
+        <v>6</v>
+      </c>
+      <c r="Z19" s="43">
+        <f t="shared" si="5"/>
+        <v>0.4075546719681909</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
-    </row>
-    <row r="21" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X20" s="43"/>
+      <c r="Z20" s="17"/>
+    </row>
+    <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>4</v>
       </c>
@@ -3837,8 +3982,18 @@
       <c r="R21" s="16" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X21" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y21" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="17">
+        <f>X21*100/100.6</f>
+        <v>2.1868787276341952</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <v>16</v>
       </c>
@@ -3875,8 +4030,18 @@
       <c r="R22" s="16" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X22" s="43">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Y22" s="16">
+        <v>17</v>
+      </c>
+      <c r="Z22" s="43">
+        <f t="shared" ref="Z22:Z34" si="9">X22*100/100.6</f>
+        <v>1.0834990059642149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>18</v>
       </c>
@@ -3913,8 +4078,18 @@
       <c r="R23" s="16" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X23" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Y23" s="16">
+        <v>2</v>
+      </c>
+      <c r="Z23" s="17">
+        <f t="shared" si="9"/>
+        <v>1.0934393638170976</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>4</v>
       </c>
@@ -3950,8 +4125,18 @@
         <f>R21</f>
         <v>L8</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X24" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y24" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z24" s="17">
+        <f t="shared" si="9"/>
+        <v>2.1868787276341952</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <v>16</v>
       </c>
@@ -3965,11 +4150,11 @@
         <v>32</v>
       </c>
       <c r="E25" s="19" t="str">
-        <f t="shared" ref="E25" si="8">RIGHT(B25,4)</f>
+        <f t="shared" ref="E25" si="10">RIGHT(B25,4)</f>
         <v>6649</v>
       </c>
       <c r="F25" s="16">
-        <f t="shared" ref="F25:F26" si="9">E25/34*35</f>
+        <f t="shared" ref="F25:F26" si="11">E25/34*35</f>
         <v>6844.5588235294117</v>
       </c>
       <c r="I25" s="19">
@@ -3987,8 +4172,18 @@
         <f>R22</f>
         <v>L16</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X25" s="43">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Y25" s="16">
+        <v>17</v>
+      </c>
+      <c r="Z25" s="43">
+        <f t="shared" si="9"/>
+        <v>1.0834990059642149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>18</v>
       </c>
@@ -4006,7 +4201,7 @@
         <v>7887</v>
       </c>
       <c r="F26" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>8118.9705882352937</v>
       </c>
       <c r="I26" s="19">
@@ -4024,8 +4219,18 @@
         <f>R23</f>
         <v>L17</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X26" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Y26" s="16">
+        <v>2</v>
+      </c>
+      <c r="Z26" s="17">
+        <f t="shared" si="9"/>
+        <v>1.0934393638170976</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A27" s="16">
         <v>4</v>
       </c>
@@ -4063,8 +4268,18 @@
         <f>R21</f>
         <v>L8</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X27" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y27" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z27" s="17">
+        <f t="shared" si="9"/>
+        <v>2.1868787276341952</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>16</v>
       </c>
@@ -4102,8 +4317,18 @@
         <f>R22</f>
         <v>L16</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X28" s="43">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Y28" s="16">
+        <v>17</v>
+      </c>
+      <c r="Z28" s="43">
+        <f t="shared" si="9"/>
+        <v>1.0834990059642149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A29" s="16">
         <v>18</v>
       </c>
@@ -4141,13 +4366,25 @@
         <f>R23</f>
         <v>L17</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" ht="12" x14ac:dyDescent="0.3">
+      <c r="X29" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Y29" s="16">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="17">
+        <f t="shared" si="9"/>
+        <v>1.0934393638170976</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="12" x14ac:dyDescent="0.3">
       <c r="M30" s="36"/>
       <c r="N30" s="36"/>
       <c r="O30" s="36"/>
-    </row>
-    <row r="31" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X30" s="43"/>
+      <c r="Z30" s="17"/>
+    </row>
+    <row r="31" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
         <v>2</v>
       </c>
@@ -4182,11 +4419,11 @@
         <v>4139.8470588235296</v>
       </c>
       <c r="K31" s="19">
-        <f t="shared" ref="J31:L33" si="10">$F31+$F$1+K$5</f>
+        <f t="shared" ref="J31:L33" si="12">$F31+$F$1+K$5</f>
         <v>5336.447058823529</v>
       </c>
       <c r="L31" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5921.7470588235301</v>
       </c>
       <c r="M31" s="37">
@@ -4221,8 +4458,18 @@
         <f>R31</f>
         <v>L4</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X31" s="43">
+        <v>8.4</v>
+      </c>
+      <c r="Y31" s="16">
+        <v>6</v>
+      </c>
+      <c r="Z31" s="43">
+        <f t="shared" si="9"/>
+        <v>8.3499005964214721</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>2</v>
       </c>
@@ -4257,11 +4504,11 @@
         <v>4899.552941176471</v>
       </c>
       <c r="K32" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6096.1529411764704</v>
       </c>
       <c r="L32" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6681.4529411764706</v>
       </c>
       <c r="M32" s="40">
@@ -4296,8 +4543,18 @@
         <f>R32</f>
         <v>L11</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X32" s="43">
+        <v>8.4</v>
+      </c>
+      <c r="Y32" s="16">
+        <v>6</v>
+      </c>
+      <c r="Z32" s="43">
+        <f t="shared" si="9"/>
+        <v>8.3499005964214721</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>2</v>
       </c>
@@ -4328,15 +4585,15 @@
         <v>84</v>
       </c>
       <c r="J33" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4519.7</v>
       </c>
       <c r="K33" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5716.2999999999993</v>
       </c>
       <c r="L33" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6301.6</v>
       </c>
       <c r="M33" s="41">
@@ -4371,8 +4628,26 @@
         <f>R33</f>
         <v>L14</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" ht="12" x14ac:dyDescent="0.3">
+      <c r="X33" s="43">
+        <v>8.4</v>
+      </c>
+      <c r="Y33" s="16">
+        <v>6</v>
+      </c>
+      <c r="Z33" s="43">
+        <f t="shared" si="9"/>
+        <v>8.3499005964214721</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="X34" s="43"/>
+      <c r="Z34" s="17"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="X35" s="43"/>
+      <c r="Z35" s="17"/>
+    </row>
+    <row r="36" spans="1:26" ht="12" x14ac:dyDescent="0.3">
       <c r="D36" s="16" t="s">
         <v>109</v>
       </c>
@@ -4387,8 +4662,10 @@
         <f>G37</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="X36" s="43"/>
+      <c r="Z36" s="17"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D37" s="32" t="s">
         <v>22</v>
       </c>
@@ -4401,8 +4678,10 @@
       <c r="G37" s="32">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="X37" s="43"/>
+      <c r="Z37" s="17"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D38" s="32" t="s">
         <v>81</v>
       </c>
@@ -4415,8 +4694,10 @@
       <c r="G38" s="32">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X38" s="43"/>
+      <c r="Z38" s="17"/>
+    </row>
+    <row r="39" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A39" s="16">
         <v>8</v>
       </c>
@@ -4463,8 +4744,18 @@
       <c r="P39" s="39" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="X39" s="43">
+        <v>4.2</v>
+      </c>
+      <c r="Y39" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z39" s="17">
+        <f t="shared" ref="Z39" si="13">X39*100/100.6</f>
+        <v>4.174950298210736</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="B40" s="16" t="s">
         <v>114</v>
       </c>
@@ -4488,7 +4779,7 @@
         <v>9058.5</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" ht="13.2" x14ac:dyDescent="0.3">
       <c r="B41" s="16" t="s">
         <v>114</v>
       </c>
@@ -4502,7 +4793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B42" s="16" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Update all adopted ENSDF files: enhance clarity, add missing sections, and ensure compliance with ordering policy.
</commit_message>
<xml_diff>
--- a/35K EC, 36Ca ECP.xlsx
+++ b/35K EC, 36Ca ECP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\A35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ACDEE0-B2AE-4E86-9941-FCD600781E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7BA670-BC27-4284-A058-9795CA2CB80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11712" yWindow="-24" windowWidth="11436" windowHeight="12000" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
   </bookViews>
   <sheets>
     <sheet name="36Ca" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="122">
   <si>
     <t>Ip</t>
   </si>
@@ -390,6 +390,18 @@
   </si>
   <si>
     <t>first p</t>
+  </si>
+  <si>
+    <t>Ip(abs)</t>
+  </si>
+  <si>
+    <t>σIp</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Table 3</t>
   </si>
 </sst>
 </file>
@@ -400,7 +412,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +559,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -569,7 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -698,6 +716,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2523,15 +2556,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82375D98-27FE-4F56-B80A-6CBF87E329ED}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="8.88671875" style="16"/>
     <col min="4" max="4" width="10.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="16"/>
+    <col min="5" max="9" width="8.88671875" style="16"/>
+    <col min="10" max="10" width="6.5546875" style="16" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -2544,6 +2579,12 @@
       <c r="E1" s="16" t="s">
         <v>15</v>
       </c>
+      <c r="G1" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="I1" s="16" t="s">
         <v>21</v>
       </c>
@@ -2837,12 +2878,15 @@
       <c r="F12" s="16">
         <v>1.8</v>
       </c>
+      <c r="I12" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="43">
         <f>SUM(E3:E12)</f>
         <v>297.7</v>
       </c>
@@ -2850,6 +2894,12 @@
         <f>SQRT(SUMSQ(F3:F12))</f>
         <v>14.25622670975739</v>
       </c>
+      <c r="I13" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D14" s="16" t="s">
@@ -2866,7 +2916,22 @@
         <v>7.3328854551561978E-4</v>
       </c>
       <c r="H14" s="26">
-        <v>1.7899999999999999E-4</v>
+        <v>3.1E-4</v>
+      </c>
+      <c r="I14" s="45">
+        <f>0.062%</f>
+        <v>6.2E-4</v>
+      </c>
+      <c r="J14" s="44">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="K14" s="46">
+        <f>I14/G14</f>
+        <v>0.84550618415025192</v>
+      </c>
+      <c r="L14" s="46">
+        <f>J14/H14</f>
+        <v>0.83870967741935476</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2878,7 +2943,21 @@
         <v>1.7524353375881761E-3</v>
       </c>
       <c r="H15" s="27">
-        <v>2.9799999999999998E-4</v>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I15" s="47">
+        <v>1.5E-3</v>
+      </c>
+      <c r="J15" s="25">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="K15" s="48">
+        <f>I15/G15</f>
+        <v>0.85595169637722834</v>
+      </c>
+      <c r="L15" s="48">
+        <f>J15/H15</f>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2991,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0A5003-67F5-4A2F-AC32-71311414C574}">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="11.4" x14ac:dyDescent="0.3"/>
@@ -3911,7 +3990,7 @@
         <v>9144.4823529411769</v>
       </c>
       <c r="M19" s="38">
-        <f t="shared" si="3"/>
+        <f>MAX(I19:L19)</f>
         <v>9144.4823529411769</v>
       </c>
       <c r="N19" s="38">
@@ -4037,7 +4116,7 @@
         <v>17</v>
       </c>
       <c r="Z22" s="43">
-        <f t="shared" ref="Z22:Z34" si="9">X22*100/100.6</f>
+        <f t="shared" ref="Z22:Z33" si="9">X22*100/100.6</f>
         <v>1.0834990059642149</v>
       </c>
     </row>

</xml_diff>